<commit_message>
App Config name changes similar to key vault
</commit_message>
<xml_diff>
--- a/CRM Solution Manager/Release/WebJob/AzureKeyVaultNames.xlsx
+++ b/CRM Solution Manager/Release/WebJob/AzureKeyVaultNames.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m-ynaresh\source\repos\DynamicsPOC3\CRM Solution Manager\Release\WebJob\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m-jkrishnan\source\repos\DynamicsPOC\CRM Solution Manager\Release\WebJob\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE85333E-A9CA-4A8B-B3EA-2A58CD38CA6F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E85ACF90-6E5E-43F2-AE7B-D85B49B0BF08}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{954886C5-4D1A-4ACB-BA8C-D15138D5C5AD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{954886C5-4D1A-4ACB-BA8C-D15138D5C5AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>ClientApplicationSecret</t>
   </si>
@@ -216,6 +216,15 @@
   </si>
   <si>
     <t xml:space="preserve">Client Secret Id of app registration,Used for Solution checker powershell task arguments in the build pipeline </t>
+  </si>
+  <si>
+    <t>BASESECRETURI</t>
+  </si>
+  <si>
+    <t>https://cicdsecretkeyvalues.vault.azure.net/</t>
+  </si>
+  <si>
+    <t>DNS value of Azure Secret key vault</t>
   </si>
 </sst>
 </file>
@@ -609,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADDD7F1C-CBB7-4AFC-820F-85C7897AE793}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -743,6 +752,17 @@
         <v>23</v>
       </c>
     </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Changes for connect crm using azure client ID
</commit_message>
<xml_diff>
--- a/CRM Solution Manager/Release/WebJob/AzureKeyVaultNames.xlsx
+++ b/CRM Solution Manager/Release/WebJob/AzureKeyVaultNames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m-jkrishnan\source\repos\DynamicsPOC\CRM Solution Manager\Release\WebJob\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E85ACF90-6E5E-43F2-AE7B-D85B49B0BF08}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1218E576-8983-4BA3-AAC2-577B837063A0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{954886C5-4D1A-4ACB-BA8C-D15138D5C5AD}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>ClientApplicationSecret</t>
   </si>
@@ -66,12 +66,6 @@
     <t>TFSUser</t>
   </si>
   <si>
-    <t>8G=kcnS2c_m9FLn5nce_:8jtHg0.:2wg</t>
-  </si>
-  <si>
-    <t>https://igdcicd2.api.crm8.dynamics.com/XRMServices/2011/Organization.svc</t>
-  </si>
-  <si>
     <t>6e%\pbw}zBySp@tY</t>
   </si>
   <si>
@@ -81,18 +75,6 @@
     <t>AuthType=Office365;Username=igdsa36@IGDCRM.onmicrosoft.com;Password=6e%\pbw}zBySp@tY;Url=https://igdcicd1.crm8.dynamics.com</t>
   </si>
   <si>
-    <t>r7swfuhp2eoq5vwjkhzjxgf7of2yxvuyobhifzpjptrfenfp2xsa</t>
-  </si>
-  <si>
-    <t>v-jaikri@microsoft.com</t>
-  </si>
-  <si>
-    <t>ebfa6cd7-c2c9-457b-a35f-743b26ddf177</t>
-  </si>
-  <si>
-    <t>72f988bf-86f1-41af-91ab-2d7cd011db47</t>
-  </si>
-  <si>
     <t>TOKENTEST</t>
   </si>
   <si>
@@ -112,9 +94,6 @@
   </si>
   <si>
     <t xml:space="preserve">Tenent Id of app registration, Used for Solution checker powershell task arguments in the build pipeline </t>
-  </si>
-  <si>
-    <t>Source D365 Instance Organization service URL</t>
   </si>
   <si>
     <t>Source D365 Instance Organization Password</t>
@@ -221,17 +200,35 @@
     <t>BASESECRETURI</t>
   </si>
   <si>
-    <t>https://cicdsecretkeyvalues.vault.azure.net/</t>
-  </si>
-  <si>
     <t>DNS value of Azure Secret key vault</t>
+  </si>
+  <si>
+    <t>horrkvma7tdpvunkaaki5erfcf2hkkb4sl4tb2k37ciqdovsh7zq</t>
+  </si>
+  <si>
+    <t>Source D365 Instance URL</t>
+  </si>
+  <si>
+    <t>https://igdcicd2.crm8.dynamics.com</t>
+  </si>
+  <si>
+    <t>d9a1b506-a006-4359-966b-696cb2dad64d</t>
+  </si>
+  <si>
+    <t>https://dd365key.vault.azure.net/</t>
+  </si>
+  <si>
+    <t>6d12e9fd-d509-4a1d-babf-40f344202c2b</t>
+  </si>
+  <si>
+    <t>2YtQ=.R9kGf3yZk1xF.U=:=Fe[4:@vil</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,6 +248,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -290,10 +300,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -304,8 +315,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -620,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADDD7F1C-CBB7-4AFC-820F-85C7897AE793}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -636,21 +654,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="30.75" thickBot="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>12</v>
+      <c r="B2" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1">
@@ -658,21 +676,21 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>14</v>
+      <c r="B4" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="60.75" thickBot="1">
@@ -680,21 +698,21 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" thickBot="1">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>16</v>
+      <c r="B6" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" thickBot="1">
@@ -702,10 +720,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30.75" thickBot="1">
@@ -713,10 +731,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30.75" thickBot="1">
@@ -724,10 +742,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" thickBot="1">
@@ -735,10 +753,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" thickBot="1">
@@ -746,25 +764,29 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{71EAD805-FFC4-4F92-82CB-6FD948AA7718}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{B49221DE-3EDB-472C-923E-431A51D37017}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>